<commit_message>
Update BOM Proposal and Options.xlsx
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/BOM Proposal and Options.xlsx
+++ b/Document Library/Bill Of Materials/BOM Proposal and Options.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{50F2830B-CDDD-493A-98A1-15A5A88378F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F91634F-C65D-4C79-8113-7A6ADBD08F7A}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{D3D6F9E7-CBEE-4761-A2BB-8F132089315E}"/>
+    <workbookView xWindow="825" yWindow="-105" windowWidth="18495" windowHeight="11025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hot Ends" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>This document contains part and component proposal and options</t>
   </si>
@@ -61,16 +56,63 @@
   </si>
   <si>
     <t>Chamber Filter</t>
+  </si>
+  <si>
+    <t>Water cooled Hot Ends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacture </t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Cost US $</t>
+  </si>
+  <si>
+    <t>Max T deg C</t>
+  </si>
+  <si>
+    <t>Silicon sock</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>TriangleLabs</t>
+  </si>
+  <si>
+    <t>Dragon Hotend  standard flow</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>Dragon Hotend  High flow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,13 +135,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,23 +457,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BE5005-1F58-4395-A22B-964D35948AC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -466,4 +519,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1">
+        <v>500</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>96</v>
+      </c>
+      <c r="E5" s="1">
+        <v>500</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>